<commit_message>
Pridan Hilluv model a treni
</commit_message>
<xml_diff>
--- a/Glenohumeral_muscles.xlsx
+++ b/Glenohumeral_muscles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoufaond\Documents\Matlab\Exoskelet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A5FD126-5A75-4A3E-BD7E-82C249F4C6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF4FAB-C11B-4B99-A125-0F6F29A628EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AB527CEB-DB72-4887-9BE2-7C54A3871F43}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="8700" xr2:uid="{AB527CEB-DB72-4887-9BE2-7C54A3871F43}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Muscle</t>
   </si>
@@ -44,9 +44,6 @@
     <t>F0M</t>
   </si>
   <si>
-    <t>Optimal_length</t>
-  </si>
-  <si>
     <t>DELT1</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>0.0832</t>
+  </si>
+  <si>
+    <t>Optimal_length_WU</t>
+  </si>
+  <si>
+    <t>Optimal_length_upravene</t>
   </si>
 </sst>
 </file>
@@ -198,8 +201,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -514,20 +518,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43E0134-3284-40C3-8FFE-7CCE759BBCC1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,150 +540,192 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>41</v>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upravene l0m jako lm pri PP
</commit_message>
<xml_diff>
--- a/Glenohumeral_muscles.xlsx
+++ b/Glenohumeral_muscles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoufaond\Documents\Matlab\Exoskelet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF4FAB-C11B-4B99-A125-0F6F29A628EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F44E1C-5157-47A9-BD9F-FE12A166E67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="8700" xr2:uid="{AB527CEB-DB72-4887-9BE2-7C54A3871F43}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Muscle</t>
   </si>
@@ -165,6 +165,45 @@
   </si>
   <si>
     <t>Optimal_length_upravene</t>
+  </si>
+  <si>
+    <t>0.152404782147249</t>
+  </si>
+  <si>
+    <t>0.0902153118932702</t>
+  </si>
+  <si>
+    <t>0.0746250795644468</t>
+  </si>
+  <si>
+    <t>0.0673973478706693</t>
+  </si>
+  <si>
+    <t>0.215514842938516</t>
+  </si>
+  <si>
+    <t>0.108857430667365</t>
+  </si>
+  <si>
+    <t>0.103602622664277</t>
+  </si>
+  <si>
+    <t>0.116559476471344</t>
+  </si>
+  <si>
+    <t>0.0418760373005853</t>
+  </si>
+  <si>
+    <t>0.103022339810354</t>
+  </si>
+  <si>
+    <t>0.0479718928123542</t>
+  </si>
+  <si>
+    <t>0.0737665405180426</t>
+  </si>
+  <si>
+    <t>0.125401365622548</t>
   </si>
 </sst>
 </file>
@@ -521,7 +560,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -568,7 +607,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -582,7 +621,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
@@ -596,7 +635,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>22</v>
@@ -610,7 +649,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>24</v>
@@ -624,7 +663,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>26</v>
@@ -638,7 +677,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>28</v>
@@ -652,7 +691,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
@@ -666,7 +705,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>32</v>
@@ -680,7 +719,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
@@ -694,7 +733,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
@@ -708,7 +747,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>38</v>
@@ -722,7 +761,7 @@
         <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>40</v>

</xml_diff>